<commit_message>
ajuste en contratos ws
</commit_message>
<xml_diff>
--- a/Definicion de servicios/ws_servidor_standAloneContratos.xlsx
+++ b/Definicion de servicios/ws_servidor_standAloneContratos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>Especificacion de servicios</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Este servicio expone una alerta donde se autoriza la entrega del dulce</t>
   </si>
   <si>
-    <t>SOAP</t>
+    <t>REST</t>
   </si>
   <si>
     <t>Request y Response (síncrono)</t>
@@ -113,6 +113,15 @@
     <t>Mensaje entregar dulce 1. Entregar Dulce 0. No entregar dulce</t>
   </si>
   <si>
+    <t>idUsuario</t>
+  </si>
+  <si>
+    <t>id del usuario que se le va a entregar el dulce</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
     <t>Este servicio se consumira cuando el dulce se entregue al "amor"</t>
   </si>
   <si>
@@ -138,6 +147,9 @@
   </si>
   <si>
     <t>Codigo de Respuesta: 1. Entregó Dulce. 0. No entregó dulce</t>
+  </si>
+  <si>
+    <t>id del usuario que se le entrego el dulce</t>
   </si>
 </sst>
 </file>
@@ -267,10 +279,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -478,8 +490,22 @@
         <v>32</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="20">
-      <c r="D20" s="11"/>
+      <c r="D20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -531,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
@@ -560,10 +586,10 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>12</v>
@@ -588,18 +614,18 @@
       <c r="D8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="F9" s="12"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -611,7 +637,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>22</v>
@@ -622,23 +648,31 @@
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10"/>
@@ -656,7 +690,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>24</v>
@@ -675,7 +709,7 @@
       <c r="A18" s="5"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="11"/>
+      <c r="D18" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>